<commit_message>
docs: update metadata reference
</commit_message>
<xml_diff>
--- a/00/RHAG00.xlsx
+++ b/00/RHAG00.xlsx
@@ -1247,42 +1247,50 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="C1" s="3" t="str">
         <v>Name</v>
       </c>
-      <c r="B1" s="3" t="str">
+      <c r="D1" s="3" t="str">
         <v>Last updated</v>
       </c>
-      <c r="C1" s="3" t="str">
-        <v>UID</v>
-      </c>
-      <c r="D1" s="3" t="str">
+      <c r="F1" s="3" t="str">
         <v>Options</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
+        <v>TdDqpX1kdd2</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>YES_NO_NUM</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <v>YES/NO (numeric)</v>
       </c>
-      <c r="B2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>TdDqpX1kdd2</v>
-      </c>
       <c r="D2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E2" s="4" t="str">
         <v>Yes; No</v>
       </c>
     </row>
@@ -1309,10 +1317,10 @@
         <v>UID</v>
       </c>
       <c r="B1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="C1" s="3" t="str">
         <v>Name</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Code</v>
       </c>
       <c r="D1" s="3" t="str">
         <v>Last updated</v>
@@ -1326,10 +1334,10 @@
         <v>Xu8ieCbS7jH</v>
       </c>
       <c r="B2" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <v>No</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>0</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
@@ -1343,10 +1351,10 @@
         <v>VavIEUmBv8j</v>
       </c>
       <c r="B3" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="str">
         <v>Yes</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>1</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
@@ -13324,7 +13332,7 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="47.7109375" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="71.7109375" customWidth="1"/>
@@ -13350,7 +13358,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>Bed density</v>
@@ -13367,7 +13375,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Incidence data</v>
@@ -13384,7 +13392,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Incidence data</v>
@@ -13401,7 +13409,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Incidence data</v>
@@ -13418,7 +13426,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Incidence data</v>
@@ -13435,7 +13443,7 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B7" s="5" t="str">
         <v>Incidence data</v>
@@ -13452,7 +13460,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Incidence data</v>
+        <v>REHAB - bed density and incidence data</v>
       </c>
       <c r="B8" s="4" t="str">
         <v>Incidence data</v>
@@ -13469,7 +13477,7 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Essential package availability</v>
+        <v>REHAB - essential package availability at PHC</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Essential package availability</v>
@@ -13486,7 +13494,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Essential package availability</v>
+        <v>REHAB - essential package availability at PHC</v>
       </c>
       <c r="B10" s="4" t="str">
         <v>Essential package availability</v>
@@ -13503,7 +13511,7 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B11" s="5" t="str">
         <v>Rehabilitation cases and sessions</v>
@@ -13520,7 +13528,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Rehabilitation cases and sessions</v>
@@ -13537,7 +13545,7 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B13" s="5" t="str">
         <v>Reabilitation service utilization</v>
@@ -13554,7 +13562,7 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B14" s="4" t="str">
         <v>Reabilitation service utilization</v>
@@ -13571,7 +13579,7 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Reabilitation service utilization</v>
@@ -13588,7 +13596,7 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B16" s="4" t="str">
         <v>Reabilitation service utilization</v>
@@ -13605,7 +13613,7 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B17" s="5" t="str">
         <v>Reabilitation service utilization</v>
@@ -13622,7 +13630,7 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B18" s="4" t="str">
         <v>Reabilitation service utilization</v>
@@ -13639,7 +13647,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B19" s="5" t="str">
         <v>Reabilitation service utilization</v>
@@ -13656,7 +13664,7 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B20" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -13673,7 +13681,7 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -13690,7 +13698,7 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B22" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -13707,7 +13715,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -13724,7 +13732,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B24" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -13741,7 +13749,7 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B25" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -13758,7 +13766,7 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B26" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -13775,7 +13783,7 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B27" s="5" t="str">
         <v>Rehabilitation facility-based uptake</v>
@@ -13792,7 +13800,7 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B28" s="4" t="str">
         <v>Assistive products</v>
@@ -13809,7 +13817,7 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>Assistive products</v>
+        <v>REHAB - inpatient report</v>
       </c>
       <c r="B29" s="5" t="str">
         <v>Assistive products</v>
@@ -13826,7 +13834,7 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B30" s="4" t="str">
         <v>Rehabilitation cases</v>
@@ -13843,7 +13851,7 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B31" s="5" t="str">
         <v>Rehabilitation cases</v>
@@ -13860,7 +13868,7 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B32" s="4" t="str">
         <v>Rehabilitation cases</v>
@@ -13877,7 +13885,7 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B33" s="5" t="str">
         <v>Rehabilitation cases</v>
@@ -13894,7 +13902,7 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B34" s="4" t="str">
         <v>Rehabilitation cases</v>
@@ -13911,7 +13919,7 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B35" s="5" t="str">
         <v>Rehabilitation cases</v>
@@ -13928,7 +13936,7 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B36" s="4" t="str">
         <v>Rehabilitation cases</v>
@@ -13945,7 +13953,7 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B37" s="5" t="str">
         <v>Rehabilitation cases</v>
@@ -13962,7 +13970,7 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B38" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -13979,7 +13987,7 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B39" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -13996,7 +14004,7 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B40" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14013,7 +14021,7 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B41" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -14030,7 +14038,7 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B42" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14047,7 +14055,7 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B43" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -14064,7 +14072,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B44" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14081,7 +14089,7 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B45" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -14098,7 +14106,7 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B46" s="4" t="str">
         <v>Rehabilitation referral</v>
@@ -14115,7 +14123,7 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B47" s="5" t="str">
         <v>Rehabilitation referral</v>
@@ -14132,7 +14140,7 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B48" s="4" t="str">
         <v>Rehabilitation facility-based uptake</v>
@@ -14149,7 +14157,7 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B49" s="5" t="str">
         <v>Rehabilitation facility-based uptake</v>
@@ -14166,7 +14174,7 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B50" s="4" t="str">
         <v>Rehabilitation facility-based uptake</v>
@@ -14183,7 +14191,7 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B51" s="5" t="str">
         <v>Assistive products</v>
@@ -14200,7 +14208,7 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B52" s="4" t="str">
         <v>Assistive products</v>
@@ -14217,7 +14225,7 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="str">
-        <v>Outreach program uptake</v>
+        <v>REHAB - outpatient report</v>
       </c>
       <c r="B53" s="5" t="str">
         <v>Outreach program uptake</v>
@@ -14234,7 +14242,7 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="str">
-        <v>Population</v>
+        <v>REHAB - personnel density</v>
       </c>
       <c r="B54" s="4" t="str">
         <v>Rehabilitation occupational groups</v>
@@ -14251,7 +14259,7 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
-        <v>Population</v>
+        <v>REHAB - personnel density</v>
       </c>
       <c r="B55" s="5" t="str">
         <v>Population</v>
@@ -14268,7 +14276,7 @@
     </row>
     <row r="56">
       <c r="A56" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B56" s="4" t="str">
         <v>Rehabilitation cases and sessions</v>
@@ -14285,7 +14293,7 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B57" s="5" t="str">
         <v>Rehabilitation cases and sessions</v>
@@ -14302,7 +14310,7 @@
     </row>
     <row r="58">
       <c r="A58" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B58" s="4" t="str">
         <v>Rehabilitation cases and sessions</v>
@@ -14319,7 +14327,7 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B59" s="5" t="str">
         <v>Rehabilitation cases and sessions</v>
@@ -14336,7 +14344,7 @@
     </row>
     <row r="60">
       <c r="A60" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B60" s="4" t="str">
         <v>Rehabilitation stay by health condition</v>
@@ -14353,7 +14361,7 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B61" s="5" t="str">
         <v>Rehabilitation stay by health condition</v>
@@ -14370,7 +14378,7 @@
     </row>
     <row r="62">
       <c r="A62" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B62" s="4" t="str">
         <v>Rehabilitation stay by health condition</v>
@@ -14387,7 +14395,7 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B63" s="5" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14404,7 +14412,7 @@
     </row>
     <row r="64">
       <c r="A64" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B64" s="4" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14421,7 +14429,7 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B65" s="5" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14438,7 +14446,7 @@
     </row>
     <row r="66">
       <c r="A66" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B66" s="4" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14455,7 +14463,7 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B67" s="5" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14472,7 +14480,7 @@
     </row>
     <row r="68">
       <c r="A68" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B68" s="4" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14489,7 +14497,7 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B69" s="5" t="str">
         <v>Rehabilitation service utilization</v>
@@ -14506,7 +14514,7 @@
     </row>
     <row r="70">
       <c r="A70" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B70" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14523,7 +14531,7 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B71" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -14540,7 +14548,7 @@
     </row>
     <row r="72">
       <c r="A72" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B72" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14557,7 +14565,7 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B73" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -14574,7 +14582,7 @@
     </row>
     <row r="74">
       <c r="A74" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B74" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14591,7 +14599,7 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B75" s="5" t="str">
         <v>Rehabilitation uptake</v>
@@ -14608,7 +14616,7 @@
     </row>
     <row r="76">
       <c r="A76" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B76" s="4" t="str">
         <v>Rehabilitation uptake</v>
@@ -14625,7 +14633,7 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B77" s="5" t="str">
         <v>Rehabilitation facility-based uptake</v>
@@ -14642,7 +14650,7 @@
     </row>
     <row r="78">
       <c r="A78" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B78" s="4" t="str">
         <v>Rehabilitation referrals</v>
@@ -14659,7 +14667,7 @@
     </row>
     <row r="79">
       <c r="A79" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B79" s="5" t="str">
         <v>Assistive products</v>
@@ -14676,7 +14684,7 @@
     </row>
     <row r="80">
       <c r="A80" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B80" s="4" t="str">
         <v>Assistive products</v>
@@ -14693,7 +14701,7 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B81" s="5" t="str">
         <v>Functioning score</v>
@@ -14710,7 +14718,7 @@
     </row>
     <row r="82">
       <c r="A82" s="4" t="str">
-        <v>Functioning score</v>
+        <v>REHAB - rehab ward report</v>
       </c>
       <c r="B82" s="4" t="str">
         <v>Functioning score</v>
@@ -14731,7 +14739,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -14746,6 +14754,7 @@
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -14779,6 +14788,9 @@
       <c r="J1" s="3" t="str">
         <v>categoryCombo Name</v>
       </c>
+      <c r="K1" s="3" t="str">
+        <v>Form Name</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
@@ -14811,6 +14823,9 @@
       <c r="J2" s="4" t="str">
         <v/>
       </c>
+      <c r="K2" s="4" t="str">
+        <v>Population</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
@@ -14843,6 +14858,9 @@
       <c r="J3" s="5" t="str">
         <v/>
       </c>
+      <c r="K3" s="5" t="str">
+        <v>Amputation incidence %</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
@@ -14875,6 +14893,9 @@
       <c r="J4" s="4" t="str">
         <v/>
       </c>
+      <c r="K4" s="4" t="str">
+        <v>Number of assistive products provided (total)</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
@@ -14907,6 +14928,9 @@
       <c r="J5" s="5" t="str">
         <v/>
       </c>
+      <c r="K5" s="5" t="str">
+        <v>Number of assistive products provided (total)</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
@@ -14939,6 +14963,9 @@
       <c r="J6" s="4" t="str">
         <v/>
       </c>
+      <c r="K6" s="4" t="str">
+        <v>Number of assistive products provided (total)</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
@@ -14971,6 +14998,9 @@
       <c r="J7" s="5" t="str">
         <v/>
       </c>
+      <c r="K7" s="5" t="str">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
@@ -15003,6 +15033,9 @@
       <c r="J8" s="4" t="str">
         <v/>
       </c>
+      <c r="K8" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
@@ -15035,6 +15068,9 @@
       <c r="J9" s="5" t="str">
         <v/>
       </c>
+      <c r="K9" s="5" t="str">
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
@@ -15067,6 +15103,9 @@
       <c r="J10" s="4" t="str">
         <v/>
       </c>
+      <c r="K10" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
@@ -15099,6 +15138,9 @@
       <c r="J11" s="5" t="str">
         <v/>
       </c>
+      <c r="K11" s="5" t="str">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
@@ -15131,6 +15173,9 @@
       <c r="J12" s="4" t="str">
         <v/>
       </c>
+      <c r="K12" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
@@ -15163,6 +15208,9 @@
       <c r="J13" s="5" t="str">
         <v/>
       </c>
+      <c r="K13" s="5" t="str">
+        <v>Total number of beds</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
@@ -15195,6 +15243,9 @@
       <c r="J14" s="4" t="str">
         <v/>
       </c>
+      <c r="K14" s="4" t="str">
+        <v>Burns incidence %</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
@@ -15227,6 +15278,9 @@
       <c r="J15" s="5" t="str">
         <v/>
       </c>
+      <c r="K15" s="5" t="str">
+        <v>Cases discharged from rehab ward</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
@@ -15259,6 +15313,9 @@
       <c r="J16" s="4" t="str">
         <v/>
       </c>
+      <c r="K16" s="4" t="str">
+        <v>First-time admissions</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
@@ -15291,6 +15348,9 @@
       <c r="J17" s="5" t="str">
         <v/>
       </c>
+      <c r="K17" s="5" t="str">
+        <v>Average functioning score at discharge</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
@@ -15323,6 +15383,9 @@
       <c r="J18" s="4" t="str">
         <v/>
       </c>
+      <c r="K18" s="4" t="str">
+        <v>Number of cases (total)</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
@@ -15355,6 +15418,9 @@
       <c r="J19" s="5" t="str">
         <v/>
       </c>
+      <c r="K19" s="5" t="str">
+        <v>Number of cases (total)</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
@@ -15387,6 +15453,9 @@
       <c r="J20" s="4" t="str">
         <v/>
       </c>
+      <c r="K20" s="4" t="str">
+        <v>Cases with cancer condition</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
@@ -15419,6 +15488,9 @@
       <c r="J21" s="5" t="str">
         <v/>
       </c>
+      <c r="K21" s="5" t="str">
+        <v>Cases with cancer condition</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
@@ -15451,6 +15523,9 @@
       <c r="J22" s="4" t="str">
         <v/>
       </c>
+      <c r="K22" s="4" t="str">
+        <v>Cases with cardiovascular condition</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
@@ -15483,6 +15558,9 @@
       <c r="J23" s="5" t="str">
         <v/>
       </c>
+      <c r="K23" s="5" t="str">
+        <v>Cases with cardiovascular condition</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
@@ -15515,6 +15593,9 @@
       <c r="J24" s="4" t="str">
         <v/>
       </c>
+      <c r="K24" s="4" t="str">
+        <v>Cases with mental condition</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
@@ -15547,6 +15628,9 @@
       <c r="J25" s="5" t="str">
         <v/>
       </c>
+      <c r="K25" s="5" t="str">
+        <v>Cases with musculoskeletal condition</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
@@ -15579,6 +15663,9 @@
       <c r="J26" s="4" t="str">
         <v/>
       </c>
+      <c r="K26" s="4" t="str">
+        <v>Cases with musculoskeletal condition</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
@@ -15611,6 +15698,9 @@
       <c r="J27" s="5" t="str">
         <v/>
       </c>
+      <c r="K27" s="5" t="str">
+        <v>Cases with respiratory condition</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
@@ -15643,6 +15733,9 @@
       <c r="J28" s="4" t="str">
         <v/>
       </c>
+      <c r="K28" s="4" t="str">
+        <v>Cases with respiratory condition</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
@@ -15675,6 +15768,9 @@
       <c r="J29" s="5" t="str">
         <v/>
       </c>
+      <c r="K29" s="5" t="str">
+        <v>Cases with sensory condition</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
@@ -15707,6 +15803,9 @@
       <c r="J30" s="4" t="str">
         <v/>
       </c>
+      <c r="K30" s="4" t="str">
+        <v>Cases with sensory condition</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
@@ -15739,6 +15838,9 @@
       <c r="J31" s="5" t="str">
         <v/>
       </c>
+      <c r="K31" s="5" t="str">
+        <v>Length of stay in rehab ward in days (totals)</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
@@ -15771,6 +15873,9 @@
       <c r="J32" s="4" t="str">
         <v/>
       </c>
+      <c r="K32" s="4" t="str">
+        <v>Package selected from national guidance</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
@@ -15803,6 +15908,9 @@
       <c r="J33" s="5" t="str">
         <v/>
       </c>
+      <c r="K33" s="5" t="str">
+        <v>Number of new cases</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
@@ -15835,6 +15943,9 @@
       <c r="J34" s="4" t="str">
         <v/>
       </c>
+      <c r="K34" s="4" t="str">
+        <v>Number of new cases</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
@@ -15867,6 +15978,9 @@
       <c r="J35" s="5" t="str">
         <v/>
       </c>
+      <c r="K35" s="5" t="str">
+        <v>New cases with comprehensive individualised care plan</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
@@ -15899,6 +16013,9 @@
       <c r="J36" s="4" t="str">
         <v/>
       </c>
+      <c r="K36" s="4" t="str">
+        <v>Rehabilitation personnel</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
@@ -15931,6 +16048,9 @@
       <c r="J37" s="5" t="str">
         <v/>
       </c>
+      <c r="K37" s="5" t="str">
+        <v>Occupational therapists</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
@@ -15963,6 +16083,9 @@
       <c r="J38" s="4" t="str">
         <v/>
       </c>
+      <c r="K38" s="4" t="str">
+        <v>Number of cases (total)</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
@@ -15995,6 +16118,9 @@
       <c r="J39" s="5" t="str">
         <v/>
       </c>
+      <c r="K39" s="5" t="str">
+        <v>Cases with cancer condition</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
@@ -16027,6 +16153,9 @@
       <c r="J40" s="4" t="str">
         <v/>
       </c>
+      <c r="K40" s="4" t="str">
+        <v>Cases with neurological condition</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="str">
@@ -16059,6 +16188,9 @@
       <c r="J41" s="5" t="str">
         <v/>
       </c>
+      <c r="K41" s="5" t="str">
+        <v>Cases with respiratory condition</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
@@ -16091,6 +16223,9 @@
       <c r="J42" s="4" t="str">
         <v/>
       </c>
+      <c r="K42" s="4" t="str">
+        <v>Cases with sensory condition</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="str">
@@ -16123,6 +16258,9 @@
       <c r="J43" s="5" t="str">
         <v/>
       </c>
+      <c r="K43" s="5" t="str">
+        <v>Number of outreach sessions</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
@@ -16155,6 +16293,9 @@
       <c r="J44" s="4" t="str">
         <v/>
       </c>
+      <c r="K44" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
@@ -16187,6 +16328,9 @@
       <c r="J45" s="5" t="str">
         <v/>
       </c>
+      <c r="K45" s="5" t="str">
+        <v>Physiotherapists</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
@@ -16219,6 +16363,9 @@
       <c r="J46" s="4" t="str">
         <v/>
       </c>
+      <c r="K46" s="4" t="str">
+        <v>Prosthetists/orthotists</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
@@ -16251,6 +16398,9 @@
       <c r="J47" s="5" t="str">
         <v/>
       </c>
+      <c r="K47" s="5" t="str">
+        <v>Psychologists</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
@@ -16283,6 +16433,9 @@
       <c r="J48" s="4" t="str">
         <v/>
       </c>
+      <c r="K48" s="4" t="str">
+        <v>Number of new referral cases</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="str">
@@ -16315,6 +16468,9 @@
       <c r="J49" s="5" t="str">
         <v/>
       </c>
+      <c r="K49" s="5" t="str">
+        <v>Number of new referral cases</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
@@ -16347,6 +16503,9 @@
       <c r="J50" s="4" t="str">
         <v/>
       </c>
+      <c r="K50" s="4" t="str">
+        <v>Rehabilitation doctors</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
@@ -16379,6 +16538,9 @@
       <c r="J51" s="5" t="str">
         <v/>
       </c>
+      <c r="K51" s="5" t="str">
+        <v>SCI incidence %</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="str">
@@ -16411,6 +16573,9 @@
       <c r="J52" s="4" t="str">
         <v/>
       </c>
+      <c r="K52" s="4" t="str">
+        <v>Sessions provided for patients with cancer condition</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="str">
@@ -16443,6 +16608,9 @@
       <c r="J53" s="5" t="str">
         <v/>
       </c>
+      <c r="K53" s="5" t="str">
+        <v>Sessions provided for patients with cancer condition</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="4" t="str">
@@ -16475,6 +16643,9 @@
       <c r="J54" s="4" t="str">
         <v/>
       </c>
+      <c r="K54" s="4" t="str">
+        <v>Sessions provided for patients with cancer condition</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
@@ -16507,6 +16678,9 @@
       <c r="J55" s="5" t="str">
         <v/>
       </c>
+      <c r="K55" s="5" t="str">
+        <v>Sessions provided for patients with cardiovascular condition</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="str">
@@ -16539,6 +16713,9 @@
       <c r="J56" s="4" t="str">
         <v/>
       </c>
+      <c r="K56" s="4" t="str">
+        <v>Sessions provided for patients with cardiovascular condition</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="str">
@@ -16571,6 +16748,9 @@
       <c r="J57" s="5" t="str">
         <v/>
       </c>
+      <c r="K57" s="5" t="str">
+        <v>Sessions provided (total)</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="4" t="str">
@@ -16603,6 +16783,9 @@
       <c r="J58" s="4" t="str">
         <v/>
       </c>
+      <c r="K58" s="4" t="str">
+        <v>Sessions provided (total)</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="str">
@@ -16635,6 +16818,9 @@
       <c r="J59" s="5" t="str">
         <v/>
       </c>
+      <c r="K59" s="5" t="str">
+        <v>Sessions provided for patients with mental condition</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="4" t="str">
@@ -16667,6 +16853,9 @@
       <c r="J60" s="4" t="str">
         <v/>
       </c>
+      <c r="K60" s="4" t="str">
+        <v>Sessions provided for patients with mental condition</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="str">
@@ -16699,6 +16888,9 @@
       <c r="J61" s="5" t="str">
         <v/>
       </c>
+      <c r="K61" s="5" t="str">
+        <v>Sessions provided for patients with mental condition</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="str">
@@ -16731,6 +16923,9 @@
       <c r="J62" s="4" t="str">
         <v/>
       </c>
+      <c r="K62" s="4" t="str">
+        <v>Sessions provided for patients with musculoskeletal condition</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="str">
@@ -16763,6 +16958,9 @@
       <c r="J63" s="5" t="str">
         <v/>
       </c>
+      <c r="K63" s="5" t="str">
+        <v>Sessions provided for patients with musculoskeletal condition</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="4" t="str">
@@ -16795,6 +16993,9 @@
       <c r="J64" s="4" t="str">
         <v/>
       </c>
+      <c r="K64" s="4" t="str">
+        <v>Sessions provided for patients with musculoskeletal condition</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="str">
@@ -16827,6 +17028,9 @@
       <c r="J65" s="5" t="str">
         <v/>
       </c>
+      <c r="K65" s="5" t="str">
+        <v>Sessions provided for patients with neurological condition</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="4" t="str">
@@ -16859,6 +17063,9 @@
       <c r="J66" s="4" t="str">
         <v/>
       </c>
+      <c r="K66" s="4" t="str">
+        <v>Sessions provided for patients with neurological condition</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="str">
@@ -16891,6 +17098,9 @@
       <c r="J67" s="5" t="str">
         <v/>
       </c>
+      <c r="K67" s="5" t="str">
+        <v>Number of sessions provided by</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="4" t="str">
@@ -16923,6 +17133,9 @@
       <c r="J68" s="4" t="str">
         <v/>
       </c>
+      <c r="K68" s="4" t="str">
+        <v>Sessions provided (total)</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="str">
@@ -16955,6 +17168,9 @@
       <c r="J69" s="5" t="str">
         <v/>
       </c>
+      <c r="K69" s="5" t="str">
+        <v>Sessions provided for patients with respiratory condition</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="4" t="str">
@@ -16987,6 +17203,9 @@
       <c r="J70" s="4" t="str">
         <v/>
       </c>
+      <c r="K70" s="4" t="str">
+        <v>Sessions provided for patients with respiratory condition</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="str">
@@ -17019,6 +17238,9 @@
       <c r="J71" s="5" t="str">
         <v/>
       </c>
+      <c r="K71" s="5" t="str">
+        <v>Sessions provided for patients with sensory condition</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="4" t="str">
@@ -17051,6 +17273,9 @@
       <c r="J72" s="4" t="str">
         <v/>
       </c>
+      <c r="K72" s="4" t="str">
+        <v>Speech language therapists</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="str">
@@ -17083,6 +17308,9 @@
       <c r="J73" s="5" t="str">
         <v/>
       </c>
+      <c r="K73" s="5" t="str">
+        <v>Stroke incidence %</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="4" t="str">
@@ -17115,6 +17343,9 @@
       <c r="J74" s="4" t="str">
         <v/>
       </c>
+      <c r="K74" s="4" t="str">
+        <v>Number of waiting days for the assistive product (total)</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="str">
@@ -17147,6 +17378,9 @@
       <c r="J75" s="5" t="str">
         <v/>
       </c>
+      <c r="K75" s="5" t="str">
+        <v>Number of waiting days for the assistive product (total)</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="4" t="str">
@@ -17179,6 +17413,9 @@
       <c r="J76" s="4" t="str">
         <v/>
       </c>
+      <c r="K76" s="4" t="str">
+        <v>Number of waiting days for the assistive product (total)</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="str">
@@ -17211,6 +17448,9 @@
       <c r="J77" s="5" t="str">
         <v/>
       </c>
+      <c r="K77" s="5" t="str">
+        <v>Number of first sessions provided by</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="4" t="str">
@@ -17243,6 +17483,9 @@
       <c r="J78" s="4" t="str">
         <v/>
       </c>
+      <c r="K78" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="5" t="str">
@@ -17275,6 +17518,9 @@
       <c r="J79" s="5" t="str">
         <v/>
       </c>
+      <c r="K79" s="5" t="str">
+        <v>Average functioning score at admission for discharged patients</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="4" t="str">
@@ -17307,6 +17553,9 @@
       <c r="J80" s="4" t="str">
         <v/>
       </c>
+      <c r="K80" s="4" t="str">
+        <v>Cases with mental condition</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="5" t="str">
@@ -17339,6 +17588,9 @@
       <c r="J81" s="5" t="str">
         <v/>
       </c>
+      <c r="K81" s="5" t="str">
+        <v>Cases with neurological condition</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="4" t="str">
@@ -17371,6 +17623,9 @@
       <c r="J82" s="4" t="str">
         <v/>
       </c>
+      <c r="K82" s="4" t="str">
+        <v>Cases with neurological condition</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="5" t="str">
@@ -17403,6 +17658,9 @@
       <c r="J83" s="5" t="str">
         <v/>
       </c>
+      <c r="K83" s="5" t="str">
+        <v>MMT Incidence %</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="4" t="str">
@@ -17435,6 +17693,9 @@
       <c r="J84" s="4" t="str">
         <v/>
       </c>
+      <c r="K84" s="4" t="str">
+        <v>Other</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="5" t="str">
@@ -17467,6 +17728,9 @@
       <c r="J85" s="5" t="str">
         <v/>
       </c>
+      <c r="K85" s="5" t="str">
+        <v>Cases with cardiovascular condition</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="4" t="str">
@@ -17499,6 +17763,9 @@
       <c r="J86" s="4" t="str">
         <v/>
       </c>
+      <c r="K86" s="4" t="str">
+        <v>Cases with mental condition</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="5" t="str">
@@ -17531,6 +17798,9 @@
       <c r="J87" s="5" t="str">
         <v/>
       </c>
+      <c r="K87" s="5" t="str">
+        <v>Cases with musculoskeletal condition</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="4" t="str">
@@ -17563,6 +17833,9 @@
       <c r="J88" s="4" t="str">
         <v/>
       </c>
+      <c r="K88" s="4" t="str">
+        <v>Sessions provided for patients with cardiovascular condition</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="5" t="str">
@@ -17595,6 +17868,9 @@
       <c r="J89" s="5" t="str">
         <v/>
       </c>
+      <c r="K89" s="5" t="str">
+        <v>Sessions provided by</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="4" t="str">
@@ -17627,6 +17903,9 @@
       <c r="J90" s="4" t="str">
         <v/>
       </c>
+      <c r="K90" s="4" t="str">
+        <v>Sessions provided by</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="5" t="str">
@@ -17659,6 +17938,9 @@
       <c r="J91" s="5" t="str">
         <v/>
       </c>
+      <c r="K91" s="5" t="str">
+        <v>Sessions provided for patients with neurological condition</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="4" t="str">
@@ -17691,6 +17973,9 @@
       <c r="J92" s="4" t="str">
         <v/>
       </c>
+      <c r="K92" s="4" t="str">
+        <v>Sessions provided for patients with respiratory condition</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="5" t="str">
@@ -17723,6 +18008,9 @@
       <c r="J93" s="5" t="str">
         <v/>
       </c>
+      <c r="K93" s="5" t="str">
+        <v>Sessions provided for patients with sensory condition</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="4" t="str">
@@ -17755,6 +18043,9 @@
       <c r="J94" s="4" t="str">
         <v/>
       </c>
+      <c r="K94" s="4" t="str">
+        <v>Sessions provided for patients with sensory condition</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="5" t="str">
@@ -17787,6 +18078,9 @@
       <c r="J95" s="5" t="str">
         <v/>
       </c>
+      <c r="K95" s="5" t="str">
+        <v>TBI incidence %</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="4" t="str">
@@ -17819,6 +18113,9 @@
       <c r="J96" s="4" t="str">
         <v/>
       </c>
+      <c r="K96" s="4" t="str">
+        <v>Number of waiting days for the 1st session (total)</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="5" t="str">
@@ -17850,6 +18147,9 @@
       </c>
       <c r="J97" s="5" t="str">
         <v/>
+      </c>
+      <c r="K97" s="5" t="str">
+        <v>WHO basic package for rehab services</v>
       </c>
     </row>
   </sheetData>
@@ -18649,113 +18949,157 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
         <v>Name</v>
       </c>
-      <c r="B1" s="3" t="str">
+      <c r="C1" s="3" t="str">
         <v>Last updated</v>
       </c>
-      <c r="C1" s="3" t="str">
-        <v>UID</v>
-      </c>
       <c r="D1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="E1" s="3" t="str">
         <v>Categories</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>dataDimensionType</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
+        <v>ko7kJ4s0HYi</v>
+      </c>
+      <c r="B2" s="4" t="str">
         <v>Age and sex (Rehabilitation)</v>
       </c>
-      <c r="B2" s="4" t="str">
-        <v/>
-      </c>
       <c r="C2" s="4" t="str">
-        <v>ko7kJ4s0HYi</v>
+        <v/>
       </c>
       <c r="D2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E2" s="4" t="str">
         <v>Age (Rehabilitation); Sex</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
+        <v>zOKNYuzC99P</v>
+      </c>
+      <c r="B3" s="5" t="str">
         <v>APL and age (Rehabilitation)</v>
       </c>
-      <c r="B3" s="5" t="str">
-        <v/>
-      </c>
       <c r="C3" s="5" t="str">
-        <v>zOKNYuzC99P</v>
+        <v/>
       </c>
       <c r="D3" s="5" t="str">
+        <v>REHAB_APL_AGE</v>
+      </c>
+      <c r="E3" s="5" t="str">
         <v>Age (Rehabilitation); Rehabilitation APL</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
+        <v>bjDvmb4bfuf</v>
+      </c>
+      <c r="B4" s="4" t="str">
         <v>default</v>
       </c>
-      <c r="B4" s="4" t="str">
-        <v/>
-      </c>
       <c r="C4" s="4" t="str">
-        <v>bjDvmb4bfuf</v>
+        <v/>
       </c>
       <c r="D4" s="4" t="str">
+        <v>default</v>
+      </c>
+      <c r="E4" s="4" t="str">
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
+        <v>WWS4HnG4qGC</v>
+      </c>
+      <c r="B5" s="5" t="str">
         <v>Rehabilitation health conditions</v>
       </c>
-      <c r="B5" s="5" t="str">
-        <v/>
-      </c>
       <c r="C5" s="5" t="str">
-        <v>WWS4HnG4qGC</v>
+        <v/>
       </c>
       <c r="D5" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E5" s="5" t="str">
         <v>Rehabilitation health conditions</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
+        <v>uurBibNDwhs</v>
+      </c>
+      <c r="B6" s="4" t="str">
         <v>Rehabilitation personnel</v>
       </c>
-      <c r="B6" s="4" t="str">
-        <v/>
-      </c>
       <c r="C6" s="4" t="str">
-        <v>uurBibNDwhs</v>
+        <v/>
       </c>
       <c r="D6" s="4" t="str">
+        <v>REHAB_PERS</v>
+      </c>
+      <c r="E6" s="4" t="str">
         <v>Rehabilitation occupational groups</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
+        <v>nMiZqJMTtZ7</v>
+      </c>
+      <c r="B7" s="5" t="str">
         <v>Rehabilitation services</v>
       </c>
-      <c r="B7" s="5" t="str">
-        <v/>
-      </c>
       <c r="C7" s="5" t="str">
-        <v>nMiZqJMTtZ7</v>
+        <v/>
       </c>
       <c r="D7" s="5" t="str">
+        <v>REHAB_SERVICES</v>
+      </c>
+      <c r="E7" s="5" t="str">
         <v>Rehabilitation services</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
   </sheetData>
@@ -18764,127 +19108,202 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="152.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="152.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="C1" s="3" t="str">
         <v>Name</v>
       </c>
-      <c r="B1" s="3" t="str">
+      <c r="D1" s="3" t="str">
+        <v>shortName</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Category options</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>dataDimensionType</v>
+      </c>
+      <c r="G1" s="3" t="str">
         <v>Last updated</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>UID</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>Category options</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
+        <v>cWCABxOGWjc</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>AGE_REHAB</v>
+      </c>
+      <c r="C2" s="4" t="str">
         <v>Age (Rehabilitation)</v>
       </c>
-      <c r="B2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>cWCABxOGWjc</v>
-      </c>
       <c r="D2" s="4" t="str">
+        <v>Age (Rehabilitation)</v>
+      </c>
+      <c r="E2" s="4" t="str">
         <v>0-4 years; 5-17 years; 18+ years</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="G2" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
+        <v>GLevLNI9wkl</v>
+      </c>
+      <c r="B3" s="5" t="str">
         <v>default</v>
       </c>
-      <c r="B3" s="5" t="str">
-        <v/>
-      </c>
       <c r="C3" s="5" t="str">
-        <v>GLevLNI9wkl</v>
+        <v>default</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>default</v>
       </c>
+      <c r="E3" s="5" t="str">
+        <v>default</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <v/>
+      </c>
+      <c r="G3" s="5" t="str">
+        <v>DISAGGREGATION</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
+        <v>LaUCSDrAfEM</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>REHAB_APL</v>
+      </c>
+      <c r="C4" s="4" t="str">
         <v>Rehabilitation APL</v>
       </c>
-      <c r="B4" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>LaUCSDrAfEM</v>
-      </c>
       <c r="D4" s="4" t="str">
+        <v>Rehabilitation APL</v>
+      </c>
+      <c r="E4" s="4" t="str">
         <v>Vision; Hearing; Cognition; Communication; Self-care; Mobility</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <v/>
+      </c>
+      <c r="G4" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
+        <v>Zbp5R88Wprl</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>REHAB_HEALTH_COND</v>
+      </c>
+      <c r="C5" s="5" t="str">
         <v>Rehabilitation health conditions</v>
       </c>
-      <c r="B5" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>Zbp5R88Wprl</v>
-      </c>
       <c r="D5" s="5" t="str">
+        <v>Rehabilitation health conditions</v>
+      </c>
+      <c r="E5" s="5" t="str">
         <v>SCI; TBI; Burns; Major multiple trauma; Amputation; Stroke</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <v/>
+      </c>
+      <c r="G5" s="5" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
+        <v>ePUdGQbYT6A</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>REHAB_PERS</v>
+      </c>
+      <c r="C6" s="4" t="str">
         <v>Rehabilitation occupational groups</v>
       </c>
-      <c r="B6" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>ePUdGQbYT6A</v>
-      </c>
       <c r="D6" s="4" t="str">
+        <v>Rehabilitation occupational groups</v>
+      </c>
+      <c r="E6" s="4" t="str">
         <v>Rehabilitation doctors; Physiotherapists; Occupational therapists; Speech language therapists; Prosthetists/orthotists; Psychologists; Other personnel</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <v/>
+      </c>
+      <c r="G6" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
+        <v>t73PQgK8FJv</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C7" s="5" t="str">
         <v>Rehabilitation services</v>
       </c>
-      <c r="B7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>t73PQgK8FJv</v>
-      </c>
       <c r="D7" s="5" t="str">
+        <v>Rehabilitation services</v>
+      </c>
+      <c r="E7" s="5" t="str">
         <v>Assistive products; Other rehab</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="G7" s="5" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
+        <v>FRwO58KwwJt</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v>SEX</v>
+      </c>
+      <c r="C8" s="4" t="str">
         <v>Sex</v>
       </c>
-      <c r="B8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>FRwO58KwwJt</v>
-      </c>
       <c r="D8" s="4" t="str">
+        <v>Sex</v>
+      </c>
+      <c r="E8" s="4" t="str">
         <v>Male; Female</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="G8" s="4" t="str">
+        <v>DISAGGREGATION</v>
       </c>
     </row>
   </sheetData>

</xml_diff>